<commit_message>
changes in UI and logic done
</commit_message>
<xml_diff>
--- a/Data/FBA Rates.xlsx
+++ b/Data/FBA Rates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Ayyanagouda\Last Mile Rates\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96C43A2C-3633-429A-9319-F0727FE07F28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A4662A1-CE4D-4009-ADC6-D773718DB62F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="799" activeTab="1" xr2:uid="{2A934A6A-F337-4BE5-84D4-604AD1A76B7C}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="799" activeTab="2" xr2:uid="{2A934A6A-F337-4BE5-84D4-604AD1A76B7C}"/>
   </bookViews>
   <sheets>
     <sheet name="FBA Locations (your original)" sheetId="7" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10125" uniqueCount="1858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10133" uniqueCount="1861">
   <si>
     <t>Type</t>
   </si>
@@ -5620,6 +5620,15 @@
   </si>
   <si>
     <t>Team Global</t>
+  </si>
+  <si>
+    <t>inr</t>
+  </si>
+  <si>
+    <t>PALLETIZATION</t>
+  </si>
+  <si>
+    <t>DOCUMENTATION</t>
   </si>
 </sst>
 </file>
@@ -7125,8 +7134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63453C1D-051F-4490-B686-739BEFBFD72E}">
   <dimension ref="A1:M1211"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53196,11 +53205,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17DCBAC0-BF3E-418B-AE45-66CABC3885D2}">
   <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="5" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
+      <selection pane="bottomRight" activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53804,10 +53813,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D35DF090-9BCB-459F-96DE-0C2E2C4CE155}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -53818,9 +53827,10 @@
     <col min="4" max="4" width="7.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -53840,7 +53850,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -53860,7 +53870,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>56</v>
       </c>
@@ -53871,7 +53881,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="2">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>16</v>
@@ -53880,7 +53890,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>58</v>
       </c>
@@ -53900,7 +53910,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>59</v>
       </c>
@@ -53920,7 +53930,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>59</v>
       </c>
@@ -53931,7 +53941,7 @@
         <v>15</v>
       </c>
       <c r="D6">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>16</v>
@@ -53940,7 +53950,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -53960,7 +53970,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>59</v>
       </c>
@@ -53980,7 +53990,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>59</v>
       </c>
@@ -53999,8 +54009,17 @@
       <c r="F9" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="K9" t="s">
+        <v>58</v>
+      </c>
+      <c r="L9">
+        <v>4500</v>
+      </c>
+      <c r="M9" t="s">
+        <v>1858</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>59</v>
       </c>
@@ -54019,8 +54038,17 @@
       <c r="F10" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="K10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10">
+        <v>100</v>
+      </c>
+      <c r="M10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -54039,8 +54067,17 @@
       <c r="F11" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="K11" t="s">
+        <v>1859</v>
+      </c>
+      <c r="L11">
+        <v>18</v>
+      </c>
+      <c r="M11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>56</v>
       </c>
@@ -54059,8 +54096,17 @@
       <c r="F12" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="K12" t="s">
+        <v>1860</v>
+      </c>
+      <c r="L12">
+        <v>50</v>
+      </c>
+      <c r="M12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>56</v>
       </c>
@@ -54080,7 +54126,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>56</v>
       </c>
@@ -54100,7 +54146,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -54120,7 +54166,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>56</v>
       </c>
@@ -54151,7 +54197,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -54284,23 +54330,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="b2f27841-1f59-4d8b-a7d8-14fb94542c19" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010054343BD0DD31AA4297A2EF610014A1BF" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f83d6b63ac4a176ebf43227be297d219">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b2f27841-1f59-4d8b-a7d8-14fb94542c19" xmlns:ns4="2f06b1f5-604c-4482-a64c-c80cee61fd3a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b05693fd1cbd9bcfb6d15831f4adf40f" ns3:_="" ns4:_="">
     <xsd:import namespace="b2f27841-1f59-4d8b-a7d8-14fb94542c19"/>
@@ -54521,32 +54550,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{846BEFA8-E503-43F6-8522-0715596E6C88}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b2f27841-1f59-4d8b-a7d8-14fb94542c19"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="2f06b1f5-604c-4482-a64c-c80cee61fd3a"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B4D3F6-F8FA-4C9E-92B9-9E9ABA11DC61}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="b2f27841-1f59-4d8b-a7d8-14fb94542c19" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EE1D8D6-1CF0-41FD-8D99-059178BD00EB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -54563,4 +54584,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67B4D3F6-F8FA-4C9E-92B9-9E9ABA11DC61}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{846BEFA8-E503-43F6-8522-0715596E6C88}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b2f27841-1f59-4d8b-a7d8-14fb94542c19"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="2f06b1f5-604c-4482-a64c-c80cee61fd3a"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>